<commit_message>
new changes and pages added
</commit_message>
<xml_diff>
--- a/onpassivewebinar/external_data/logindata.xlsx
+++ b/onpassivewebinar/external_data/logindata.xlsx
@@ -31,10 +31,10 @@
     <t>vijay</t>
   </si>
   <si>
-    <t>ravii.ranjan49@gmail.com</t>
-  </si>
-  <si>
-    <t>Onp@ssive90</t>
+    <t>ravi.ranjan@onpassive.com</t>
+  </si>
+  <si>
+    <t>Onpassive90@</t>
   </si>
 </sst>
 </file>

</xml_diff>